<commit_message>
Added TestCase01_1 for re-registration
</commit_message>
<xml_diff>
--- a/app/src/test/resources/DatasetsforZcommerce.xlsx
+++ b/app/src/test/resources/DatasetsforZcommerce.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Zcommerce\Zcommerce\app\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D950E5D-239A-4D33-8DFB-F9B1EAB24E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D38D37-D4BE-4519-A140-B4248578735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase01" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCase01_1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>#</t>
   </si>
@@ -368,8 +369,8 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -444,4 +445,86 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41507D13-3B13-47CF-8213-BA6D2E390C66}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{BADF4BE4-30F6-49D3-8D39-696DB2673E87}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{116F867A-F29E-4655-8227-202F1DF19BFD}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{B722385D-BE35-49CB-BE01-3CA6E0A0ED7C}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{7E0A5EEF-0862-476C-B0F7-813BCC9F1E7D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added dp in testcase02
</commit_message>
<xml_diff>
--- a/app/src/test/resources/DatasetsforZcommerce.xlsx
+++ b/app/src/test/resources/DatasetsforZcommerce.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Zcommerce\Zcommerce\app\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D38D37-D4BE-4519-A140-B4248578735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C88ADB-7468-4960-8DE8-CA87561D02A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase01" sheetId="1" r:id="rId1"/>
     <sheet name="TestCase01_1" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCase02" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>#</t>
   </si>
@@ -60,6 +61,18 @@
   </si>
   <si>
     <t>Pablo@123</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>boss</t>
+  </si>
+  <si>
+    <t>Surya</t>
+  </si>
+  <si>
+    <t>Busch</t>
   </si>
 </sst>
 </file>
@@ -451,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41507D13-3B13-47CF-8213-BA6D2E390C66}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -527,4 +540,54 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAD0AA9-12D9-41E8-806D-FB36A5085153}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>